<commit_message>
added episodes to experiment
</commit_message>
<xml_diff>
--- a/metrics/tables/sac.xlsx
+++ b/metrics/tables/sac.xlsx
@@ -455,10 +455,10 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.3006150128336459</v>
+        <v>-0.876623476148397</v>
       </c>
       <c r="B3" t="n">
-        <v>0.02261695597577795</v>
+        <v>-1.154621533006265</v>
       </c>
     </row>
     <row r="4">
@@ -503,10 +503,10 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.2791394166518081</v>
+        <v>0.2752495366249035</v>
       </c>
       <c r="B9" t="n">
-        <v>0.001141359793940089</v>
+        <v>-0.002748520232964513</v>
       </c>
     </row>
     <row r="10">

</xml_diff>